<commit_message>
use of "*.md" and pandas_dataframe
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -35,16 +35,16 @@
     <t xml:space="preserve">rejeita-se</t>
   </si>
   <si>
+    <t xml:space="preserve">é maior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">é significativamente maior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">não se rejeita</t>
+  </si>
+  <si>
     <t xml:space="preserve">é menor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">é significativamente maior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">não se rejeita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">é maior</t>
   </si>
   <si>
     <t xml:space="preserve">não é significativamente maior</t>

</xml_diff>